<commit_message>
1.amount from Double to BigDecimal 2.refactoring method createOffer
</commit_message>
<xml_diff>
--- a/reports/users.xlsx
+++ b/reports/users.xlsx
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="49">
   <si>
     <t>Users</t>
   </si>
@@ -150,6 +150,33 @@
   </si>
   <si>
     <t>Mauritania</t>
+  </si>
+  <si>
+    <t>70000008066</t>
+  </si>
+  <si>
+    <t>UwLyX+test@RCB.com</t>
+  </si>
+  <si>
+    <t>Australia</t>
+  </si>
+  <si>
+    <t>70000028174</t>
+  </si>
+  <si>
+    <t>yFsOM+test@ZRN.com</t>
+  </si>
+  <si>
+    <t>70000014689</t>
+  </si>
+  <si>
+    <t>bELDl+test@FPP.com</t>
+  </si>
+  <si>
+    <t>70000011098</t>
+  </si>
+  <si>
+    <t>qgsEZ+test@sTT.com</t>
   </si>
 </sst>
 </file>
@@ -503,7 +530,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BD98A14D-B425-C945-9937-30EF5E4DE984}">
-  <dimension ref="A1:F13"/>
+  <dimension ref="A1:F17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="E18" sqref="E18"/>
@@ -726,6 +753,74 @@
         <v>39</v>
       </c>
     </row>
+    <row r="14">
+      <c r="B14" t="s">
+        <v>6</v>
+      </c>
+      <c r="C14" t="s">
+        <v>40</v>
+      </c>
+      <c r="D14" t="s">
+        <v>41</v>
+      </c>
+      <c r="E14" t="s">
+        <v>4</v>
+      </c>
+      <c r="F14" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="B15" t="s">
+        <v>6</v>
+      </c>
+      <c r="C15" t="s">
+        <v>43</v>
+      </c>
+      <c r="D15" t="s">
+        <v>44</v>
+      </c>
+      <c r="E15" t="s">
+        <v>4</v>
+      </c>
+      <c r="F15" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="B16" t="s">
+        <v>6</v>
+      </c>
+      <c r="C16" t="s">
+        <v>45</v>
+      </c>
+      <c r="D16" t="s">
+        <v>46</v>
+      </c>
+      <c r="E16" t="s">
+        <v>4</v>
+      </c>
+      <c r="F16" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="B17" t="s">
+        <v>6</v>
+      </c>
+      <c r="C17" t="s">
+        <v>47</v>
+      </c>
+      <c r="D17" t="s">
+        <v>48</v>
+      </c>
+      <c r="E17" t="s">
+        <v>4</v>
+      </c>
+      <c r="F17" t="s">
+        <v>42</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>

</xml_diff>

<commit_message>
Test for Australian users Test Bank transfer, Voucher, TopUp Mobile Refactoring
</commit_message>
<xml_diff>
--- a/reports/users.xlsx
+++ b/reports/users.xlsx
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="56">
   <si>
     <t>Users</t>
   </si>
@@ -177,6 +177,27 @@
   </si>
   <si>
     <t>qgsEZ+test@sTT.com</t>
+  </si>
+  <si>
+    <t>70000017358</t>
+  </si>
+  <si>
+    <t>uxnvH+test@ogJ.com</t>
+  </si>
+  <si>
+    <t>70000019235</t>
+  </si>
+  <si>
+    <t>qUImP+test@Zcb.com</t>
+  </si>
+  <si>
+    <t>PROD</t>
+  </si>
+  <si>
+    <t>70000027021</t>
+  </si>
+  <si>
+    <t>jtAgW+test@nyb.com</t>
   </si>
 </sst>
 </file>
@@ -530,7 +551,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BD98A14D-B425-C945-9937-30EF5E4DE984}">
-  <dimension ref="A1:F17"/>
+  <dimension ref="A1:F20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="E18" sqref="E18"/>
@@ -821,6 +842,57 @@
         <v>42</v>
       </c>
     </row>
+    <row r="18">
+      <c r="B18" t="s">
+        <v>6</v>
+      </c>
+      <c r="C18" t="s">
+        <v>49</v>
+      </c>
+      <c r="D18" t="s">
+        <v>50</v>
+      </c>
+      <c r="E18" t="s">
+        <v>4</v>
+      </c>
+      <c r="F18" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="B19" t="s">
+        <v>6</v>
+      </c>
+      <c r="C19" t="s">
+        <v>51</v>
+      </c>
+      <c r="D19" t="s">
+        <v>52</v>
+      </c>
+      <c r="E19" t="s">
+        <v>4</v>
+      </c>
+      <c r="F19" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="B20" t="s">
+        <v>53</v>
+      </c>
+      <c r="C20" t="s">
+        <v>54</v>
+      </c>
+      <c r="D20" t="s">
+        <v>55</v>
+      </c>
+      <c r="E20" t="s">
+        <v>4</v>
+      </c>
+      <c r="F20" t="s">
+        <v>42</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>

</xml_diff>

<commit_message>
separated urls for MANAGEMENT, MOBILE and KYC
</commit_message>
<xml_diff>
--- a/reports/users.xlsx
+++ b/reports/users.xlsx
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="364" uniqueCount="194">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="419" uniqueCount="223">
   <si>
     <t>Users</t>
   </si>
@@ -612,6 +612,93 @@
   </si>
   <si>
     <t>cKjBN+test@xSZ.com</t>
+  </si>
+  <si>
+    <t>PROD</t>
+  </si>
+  <si>
+    <t>70000016930</t>
+  </si>
+  <si>
+    <t>fJUGR+test@QUE.com</t>
+  </si>
+  <si>
+    <t>70000023280</t>
+  </si>
+  <si>
+    <t>cPVBI+test@EnN.com</t>
+  </si>
+  <si>
+    <t>70000020910</t>
+  </si>
+  <si>
+    <t>lNUKj+test@zez.com</t>
+  </si>
+  <si>
+    <t>70000014055</t>
+  </si>
+  <si>
+    <t>SctRi+test@MWW.com</t>
+  </si>
+  <si>
+    <t>70000022662</t>
+  </si>
+  <si>
+    <t>Mznte+test@eRI.com</t>
+  </si>
+  <si>
+    <t>Afghanistan</t>
+  </si>
+  <si>
+    <t>70000000075</t>
+  </si>
+  <si>
+    <t>ZbaYq+test@Gha.com</t>
+  </si>
+  <si>
+    <t>Belarus</t>
+  </si>
+  <si>
+    <t>70000003377</t>
+  </si>
+  <si>
+    <t>SagPQ+test@OaY.com</t>
+  </si>
+  <si>
+    <t>Gambia</t>
+  </si>
+  <si>
+    <t>70000012537</t>
+  </si>
+  <si>
+    <t>fEjpl+test@ROK.com</t>
+  </si>
+  <si>
+    <t>Madagascar</t>
+  </si>
+  <si>
+    <t>70000010966</t>
+  </si>
+  <si>
+    <t>fRXLL+test@mmt.com</t>
+  </si>
+  <si>
+    <t>Cyprus</t>
+  </si>
+  <si>
+    <t>70000024340</t>
+  </si>
+  <si>
+    <t>gtuvH+test@PmZ.com</t>
+  </si>
+  <si>
+    <t>Egypt</t>
+  </si>
+  <si>
+    <t>70000003311</t>
+  </si>
+  <si>
+    <t>EPhQr+test@XRP.com</t>
   </si>
 </sst>
 </file>
@@ -965,7 +1052,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BD98A14D-B425-C945-9937-30EF5E4DE984}">
-  <dimension ref="A1:G73"/>
+  <dimension ref="A1:G84"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection sqref="A1:G17"/>
@@ -2218,6 +2305,193 @@
         <v>133</v>
       </c>
     </row>
+    <row r="74">
+      <c r="B74" t="s">
+        <v>194</v>
+      </c>
+      <c r="C74" t="s">
+        <v>195</v>
+      </c>
+      <c r="D74" t="s">
+        <v>196</v>
+      </c>
+      <c r="E74" t="s">
+        <v>4</v>
+      </c>
+      <c r="F74" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="75">
+      <c r="B75" t="s">
+        <v>6</v>
+      </c>
+      <c r="C75" t="s">
+        <v>197</v>
+      </c>
+      <c r="D75" t="s">
+        <v>198</v>
+      </c>
+      <c r="E75" t="s">
+        <v>4</v>
+      </c>
+      <c r="F75" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="76">
+      <c r="B76" t="s">
+        <v>6</v>
+      </c>
+      <c r="C76" t="s">
+        <v>199</v>
+      </c>
+      <c r="D76" t="s">
+        <v>200</v>
+      </c>
+      <c r="E76" t="s">
+        <v>4</v>
+      </c>
+      <c r="F76" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="77">
+      <c r="B77" t="s">
+        <v>6</v>
+      </c>
+      <c r="C77" t="s">
+        <v>201</v>
+      </c>
+      <c r="D77" t="s">
+        <v>202</v>
+      </c>
+      <c r="E77" t="s">
+        <v>4</v>
+      </c>
+      <c r="F77" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="78">
+      <c r="B78" t="s">
+        <v>6</v>
+      </c>
+      <c r="C78" t="s">
+        <v>203</v>
+      </c>
+      <c r="D78" t="s">
+        <v>204</v>
+      </c>
+      <c r="E78" t="s">
+        <v>4</v>
+      </c>
+      <c r="F78" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="79">
+      <c r="B79" t="s">
+        <v>194</v>
+      </c>
+      <c r="C79" t="s">
+        <v>206</v>
+      </c>
+      <c r="D79" t="s">
+        <v>207</v>
+      </c>
+      <c r="E79" t="s">
+        <v>4</v>
+      </c>
+      <c r="F79" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="80">
+      <c r="B80" t="s">
+        <v>6</v>
+      </c>
+      <c r="C80" t="s">
+        <v>209</v>
+      </c>
+      <c r="D80" t="s">
+        <v>210</v>
+      </c>
+      <c r="E80" t="s">
+        <v>4</v>
+      </c>
+      <c r="F80" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="81">
+      <c r="B81" t="s">
+        <v>6</v>
+      </c>
+      <c r="C81" t="s">
+        <v>212</v>
+      </c>
+      <c r="D81" t="s">
+        <v>213</v>
+      </c>
+      <c r="E81" t="s">
+        <v>4</v>
+      </c>
+      <c r="F81" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="82">
+      <c r="B82" t="s">
+        <v>6</v>
+      </c>
+      <c r="C82" t="s">
+        <v>215</v>
+      </c>
+      <c r="D82" t="s">
+        <v>216</v>
+      </c>
+      <c r="E82" t="s">
+        <v>4</v>
+      </c>
+      <c r="F82" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="83">
+      <c r="B83" t="s">
+        <v>194</v>
+      </c>
+      <c r="C83" t="s">
+        <v>218</v>
+      </c>
+      <c r="D83" t="s">
+        <v>219</v>
+      </c>
+      <c r="E83" t="s">
+        <v>4</v>
+      </c>
+      <c r="F83" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="84">
+      <c r="B84" t="s">
+        <v>6</v>
+      </c>
+      <c r="C84" t="s">
+        <v>221</v>
+      </c>
+      <c r="D84" t="s">
+        <v>222</v>
+      </c>
+      <c r="E84" t="s">
+        <v>4</v>
+      </c>
+      <c r="F84" t="s">
+        <v>189</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>

</xml_diff>

<commit_message>
some tests added to ignore fixed invoice tests
</commit_message>
<xml_diff>
--- a/reports/users.xlsx
+++ b/reports/users.xlsx
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="419" uniqueCount="223">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="425" uniqueCount="226">
   <si>
     <t>Users</t>
   </si>
@@ -699,6 +699,15 @@
   </si>
   <si>
     <t>EPhQr+test@XRP.com</t>
+  </si>
+  <si>
+    <t>70000003601</t>
+  </si>
+  <si>
+    <t>HHzlF+test@cyi.com</t>
+  </si>
+  <si>
+    <t>88cf812c-5512-4c40-9a3d-95170336f46a</t>
   </si>
 </sst>
 </file>
@@ -1052,7 +1061,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BD98A14D-B425-C945-9937-30EF5E4DE984}">
-  <dimension ref="A1:G84"/>
+  <dimension ref="A1:G85"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection sqref="A1:G17"/>
@@ -2492,6 +2501,26 @@
         <v>189</v>
       </c>
     </row>
+    <row r="85">
+      <c r="B85" t="s">
+        <v>6</v>
+      </c>
+      <c r="C85" t="s">
+        <v>223</v>
+      </c>
+      <c r="D85" t="s">
+        <v>224</v>
+      </c>
+      <c r="E85" t="s">
+        <v>4</v>
+      </c>
+      <c r="F85" t="s">
+        <v>42</v>
+      </c>
+      <c r="G85" t="s">
+        <v>225</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>

</xml_diff>